<commit_message>
Asignación de recursos Mat 9 tema 5
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion05/ESCALETA_MA_09_05_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion05/ESCALETA_MA_09_05_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion05\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
@@ -13,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$31</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="259">
   <si>
     <t>Asignatura</t>
   </si>
@@ -781,6 +786,24 @@
   </si>
   <si>
     <t>Diaporama F1</t>
+  </si>
+  <si>
+    <t>Jairo</t>
+  </si>
+  <si>
+    <t>Johanna Montejo</t>
+  </si>
+  <si>
+    <t>Luisa</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Clara Melo</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
   </si>
 </sst>
 </file>
@@ -1086,16 +1109,49 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1131,50 +1187,17 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,7 +1259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1271,7 +1294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1482,9 +1505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:O2"/>
+      <selection pane="bottomLeft" activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,7 +1518,7 @@
     <col min="4" max="4" width="41" style="18" customWidth="1"/>
     <col min="5" max="5" width="31" style="18" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="55.85546875" style="67" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" style="42" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="17" customWidth="1"/>
     <col min="9" max="9" width="11" style="17" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" style="18" customWidth="1"/>
@@ -1503,106 +1526,107 @@
     <col min="12" max="12" width="17.42578125" style="18" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" style="18" customWidth="1"/>
     <col min="14" max="14" width="21.5703125" style="18" customWidth="1"/>
-    <col min="15" max="15" width="73.5703125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="37" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="17" customWidth="1"/>
-    <col min="18" max="18" width="23" style="18" customWidth="1"/>
-    <col min="19" max="19" width="35" style="18" customWidth="1"/>
+    <col min="15" max="15" width="73.5703125" style="17" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="37" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="17" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="23" style="18" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="35" style="18" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="25.85546875" style="18" customWidth="1"/>
     <col min="21" max="21" width="21.7109375" style="18" customWidth="1"/>
-    <col min="22" max="24" width="11.42578125" style="17"/>
+    <col min="22" max="22" width="15.7109375" style="17" customWidth="1"/>
+    <col min="23" max="24" width="11.42578125" style="17"/>
     <col min="25" max="16384" width="11.42578125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="40" t="s">
+      <c r="N1" s="63"/>
+      <c r="O1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="Q1" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="59" t="s">
+      <c r="R1" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="S1" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="57" t="s">
+      <c r="T1" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="55" t="s">
+      <c r="U1" s="45" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="47"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="58"/>
       <c r="M2" s="15" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="56"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="46"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="46"/>
     </row>
     <row r="3" spans="1:24" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1619,7 +1643,7 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="64" t="s">
+      <c r="G3" s="39" t="s">
         <v>124</v>
       </c>
       <c r="H3" s="11">
@@ -1654,13 +1678,15 @@
       <c r="S3" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="T3" s="61" t="s">
+      <c r="T3" s="38" t="s">
         <v>216</v>
       </c>
       <c r="U3" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="V3" s="16"/>
+      <c r="V3" s="17" t="s">
+        <v>255</v>
+      </c>
       <c r="W3" s="16"/>
       <c r="X3" s="16"/>
     </row>
@@ -1679,7 +1705,7 @@
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="26"/>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="40" t="s">
         <v>125</v>
       </c>
       <c r="H4" s="27">
@@ -1716,13 +1742,15 @@
       <c r="S4" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T4" s="61" t="s">
+      <c r="T4" s="38" t="s">
         <v>220</v>
       </c>
       <c r="U4" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V4" s="16"/>
+      <c r="V4" s="17" t="s">
+        <v>253</v>
+      </c>
       <c r="W4" s="16"/>
       <c r="X4" s="16"/>
     </row>
@@ -1741,7 +1769,7 @@
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="26"/>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="40" t="s">
         <v>126</v>
       </c>
       <c r="H5" s="11">
@@ -1778,13 +1806,15 @@
       <c r="S5" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T5" s="61" t="s">
+      <c r="T5" s="38" t="s">
         <v>222</v>
       </c>
       <c r="U5" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V5" s="16"/>
+      <c r="V5" s="17" t="s">
+        <v>253</v>
+      </c>
       <c r="W5" s="16"/>
       <c r="X5" s="16"/>
     </row>
@@ -1803,7 +1833,7 @@
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="26"/>
-      <c r="G6" s="65" t="s">
+      <c r="G6" s="40" t="s">
         <v>127</v>
       </c>
       <c r="H6" s="27">
@@ -1840,13 +1870,15 @@
       <c r="S6" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="T6" s="61" t="s">
+      <c r="T6" s="38" t="s">
         <v>224</v>
       </c>
       <c r="U6" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="V6" s="16"/>
+      <c r="V6" s="17" t="s">
+        <v>255</v>
+      </c>
       <c r="W6" s="16"/>
       <c r="X6" s="16"/>
     </row>
@@ -1865,7 +1897,7 @@
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="26"/>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="40" t="s">
         <v>128</v>
       </c>
       <c r="H7" s="11">
@@ -1902,13 +1934,15 @@
       <c r="S7" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="T7" s="61" t="s">
+      <c r="T7" s="38" t="s">
         <v>228</v>
       </c>
       <c r="U7" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="V7" s="16"/>
+      <c r="V7" s="17" t="s">
+        <v>253</v>
+      </c>
       <c r="W7" s="16"/>
       <c r="X7" s="16"/>
     </row>
@@ -1927,7 +1961,7 @@
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="26"/>
-      <c r="G8" s="65" t="s">
+      <c r="G8" s="40" t="s">
         <v>129</v>
       </c>
       <c r="H8" s="27">
@@ -1960,13 +1994,15 @@
       <c r="S8" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="T8" s="61" t="s">
+      <c r="T8" s="38" t="s">
         <v>129</v>
       </c>
       <c r="U8" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="V8" s="16"/>
+      <c r="V8" s="17" t="s">
+        <v>255</v>
+      </c>
       <c r="W8" s="16"/>
       <c r="X8" s="16"/>
     </row>
@@ -1985,7 +2021,7 @@
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="26"/>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="40" t="s">
         <v>130</v>
       </c>
       <c r="H9" s="11">
@@ -2020,13 +2056,15 @@
       <c r="S9" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="T9" s="61" t="s">
+      <c r="T9" s="38" t="s">
         <v>230</v>
       </c>
       <c r="U9" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="V9" s="16"/>
+      <c r="V9" s="17" t="s">
+        <v>255</v>
+      </c>
       <c r="W9" s="16"/>
       <c r="X9" s="16"/>
     </row>
@@ -2045,7 +2083,7 @@
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="26"/>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="40" t="s">
         <v>131</v>
       </c>
       <c r="H10" s="27">
@@ -2082,13 +2120,15 @@
       <c r="S10" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T10" s="61" t="s">
+      <c r="T10" s="38" t="s">
         <v>231</v>
       </c>
       <c r="U10" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V10" s="16"/>
+      <c r="V10" s="17" t="s">
+        <v>253</v>
+      </c>
       <c r="W10" s="16"/>
       <c r="X10" s="16"/>
     </row>
@@ -2107,7 +2147,7 @@
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="40" t="s">
         <v>132</v>
       </c>
       <c r="H11" s="11">
@@ -2144,13 +2184,15 @@
       <c r="S11" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T11" s="61" t="s">
+      <c r="T11" s="38" t="s">
         <v>232</v>
       </c>
       <c r="U11" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V11" s="16"/>
+      <c r="V11" s="17" t="s">
+        <v>253</v>
+      </c>
       <c r="W11" s="16"/>
       <c r="X11" s="16"/>
     </row>
@@ -2171,7 +2213,7 @@
         <v>180</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="65" t="s">
+      <c r="G12" s="40" t="s">
         <v>133</v>
       </c>
       <c r="H12" s="27">
@@ -2206,13 +2248,15 @@
       <c r="S12" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="T12" s="61" t="s">
+      <c r="T12" s="38" t="s">
         <v>233</v>
       </c>
       <c r="U12" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="V12" s="16"/>
+      <c r="V12" s="17" t="s">
+        <v>255</v>
+      </c>
       <c r="W12" s="16"/>
       <c r="X12" s="16"/>
     </row>
@@ -2231,7 +2275,7 @@
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="26"/>
-      <c r="G13" s="65" t="s">
+      <c r="G13" s="40" t="s">
         <v>134</v>
       </c>
       <c r="H13" s="11">
@@ -2268,13 +2312,15 @@
       <c r="S13" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="T13" s="61" t="s">
+      <c r="T13" s="38" t="s">
         <v>234</v>
       </c>
       <c r="U13" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="V13" s="16"/>
+      <c r="V13" s="17" t="s">
+        <v>254</v>
+      </c>
       <c r="W13" s="16"/>
       <c r="X13" s="16"/>
     </row>
@@ -2293,7 +2339,7 @@
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="26"/>
-      <c r="G14" s="65" t="s">
+      <c r="G14" s="40" t="s">
         <v>135</v>
       </c>
       <c r="H14" s="27">
@@ -2330,13 +2376,15 @@
       <c r="S14" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T14" s="61" t="s">
+      <c r="T14" s="38" t="s">
         <v>235</v>
       </c>
       <c r="U14" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V14" s="16"/>
+      <c r="V14" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="W14" s="16"/>
       <c r="X14" s="16"/>
     </row>
@@ -2355,7 +2403,7 @@
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="26"/>
-      <c r="G15" s="65" t="s">
+      <c r="G15" s="40" t="s">
         <v>136</v>
       </c>
       <c r="H15" s="11">
@@ -2392,13 +2440,15 @@
       <c r="S15" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T15" s="61" t="s">
+      <c r="T15" s="38" t="s">
         <v>236</v>
       </c>
       <c r="U15" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V15" s="16"/>
+      <c r="V15" s="17" t="s">
+        <v>254</v>
+      </c>
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
     </row>
@@ -2417,7 +2467,7 @@
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="26"/>
-      <c r="G16" s="65" t="s">
+      <c r="G16" s="40" t="s">
         <v>137</v>
       </c>
       <c r="H16" s="27">
@@ -2454,13 +2504,15 @@
       <c r="S16" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T16" s="61" t="s">
+      <c r="T16" s="38" t="s">
         <v>237</v>
       </c>
       <c r="U16" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V16" s="16"/>
+      <c r="V16" s="17" t="s">
+        <v>254</v>
+      </c>
       <c r="W16" s="16"/>
       <c r="X16" s="16"/>
     </row>
@@ -2479,7 +2531,7 @@
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
-      <c r="G17" s="65" t="s">
+      <c r="G17" s="40" t="s">
         <v>138</v>
       </c>
       <c r="H17" s="11">
@@ -2516,13 +2568,15 @@
       <c r="S17" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T17" s="61" t="s">
+      <c r="T17" s="38" t="s">
         <v>238</v>
       </c>
       <c r="U17" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V17" s="16"/>
+      <c r="V17" s="17" t="s">
+        <v>254</v>
+      </c>
       <c r="W17" s="16"/>
       <c r="X17" s="16"/>
     </row>
@@ -2541,7 +2595,7 @@
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="40" t="s">
         <v>139</v>
       </c>
       <c r="H18" s="27">
@@ -2578,13 +2632,15 @@
       <c r="S18" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T18" s="61" t="s">
+      <c r="T18" s="38" t="s">
         <v>239</v>
       </c>
       <c r="U18" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V18" s="16"/>
+      <c r="V18" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
     </row>
@@ -2603,7 +2659,7 @@
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
-      <c r="G19" s="65" t="s">
+      <c r="G19" s="40" t="s">
         <v>140</v>
       </c>
       <c r="H19" s="11">
@@ -2640,13 +2696,15 @@
       <c r="S19" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T19" s="61" t="s">
+      <c r="T19" s="38" t="s">
         <v>240</v>
       </c>
       <c r="U19" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V19" s="16"/>
+      <c r="V19" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="W19" s="16"/>
       <c r="X19" s="16"/>
     </row>
@@ -2665,7 +2723,7 @@
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="26"/>
-      <c r="G20" s="65" t="s">
+      <c r="G20" s="40" t="s">
         <v>141</v>
       </c>
       <c r="H20" s="27">
@@ -2702,13 +2760,15 @@
       <c r="S20" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T20" s="61" t="s">
+      <c r="T20" s="38" t="s">
         <v>241</v>
       </c>
       <c r="U20" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V20" s="16"/>
+      <c r="V20" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
     </row>
@@ -2727,7 +2787,7 @@
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
-      <c r="G21" s="65" t="s">
+      <c r="G21" s="40" t="s">
         <v>142</v>
       </c>
       <c r="H21" s="11">
@@ -2764,13 +2824,15 @@
       <c r="S21" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T21" s="61" t="s">
+      <c r="T21" s="38" t="s">
         <v>242</v>
       </c>
       <c r="U21" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V21" s="16"/>
+      <c r="V21" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="W21" s="16"/>
       <c r="X21" s="16"/>
     </row>
@@ -2791,7 +2853,7 @@
         <v>180</v>
       </c>
       <c r="F22" s="26"/>
-      <c r="G22" s="65" t="s">
+      <c r="G22" s="40" t="s">
         <v>143</v>
       </c>
       <c r="H22" s="27">
@@ -2828,13 +2890,15 @@
       <c r="S22" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T22" s="61" t="s">
+      <c r="T22" s="38" t="s">
         <v>243</v>
       </c>
       <c r="U22" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V22" s="16"/>
+      <c r="V22" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="W22" s="16"/>
       <c r="X22" s="16"/>
     </row>
@@ -2853,7 +2917,7 @@
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
-      <c r="G23" s="65" t="s">
+      <c r="G23" s="40" t="s">
         <v>144</v>
       </c>
       <c r="H23" s="11">
@@ -2890,13 +2954,15 @@
       <c r="S23" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="T23" s="61" t="s">
+      <c r="T23" s="38" t="s">
         <v>244</v>
       </c>
       <c r="U23" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="V23" s="16"/>
+      <c r="V23" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="W23" s="16"/>
       <c r="X23" s="16"/>
     </row>
@@ -2915,7 +2981,7 @@
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="26"/>
-      <c r="G24" s="65" t="s">
+      <c r="G24" s="40" t="s">
         <v>145</v>
       </c>
       <c r="H24" s="27">
@@ -2952,13 +3018,15 @@
       <c r="S24" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T24" s="61" t="s">
+      <c r="T24" s="38" t="s">
         <v>245</v>
       </c>
       <c r="U24" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V24" s="16"/>
+      <c r="V24" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="W24" s="16"/>
       <c r="X24" s="16"/>
     </row>
@@ -2977,7 +3045,7 @@
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="26"/>
-      <c r="G25" s="65" t="s">
+      <c r="G25" s="40" t="s">
         <v>146</v>
       </c>
       <c r="H25" s="11">
@@ -3014,13 +3082,15 @@
       <c r="S25" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T25" s="61" t="s">
+      <c r="T25" s="38" t="s">
         <v>246</v>
       </c>
       <c r="U25" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V25" s="16"/>
+      <c r="V25" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="W25" s="16"/>
       <c r="X25" s="16"/>
     </row>
@@ -3039,7 +3109,7 @@
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
-      <c r="G26" s="65" t="s">
+      <c r="G26" s="40" t="s">
         <v>178</v>
       </c>
       <c r="H26" s="27">
@@ -3076,13 +3146,15 @@
       <c r="S26" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T26" s="61" t="s">
+      <c r="T26" s="38" t="s">
         <v>247</v>
       </c>
       <c r="U26" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V26" s="16"/>
+      <c r="V26" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="W26" s="16"/>
       <c r="X26" s="16"/>
     </row>
@@ -3103,7 +3175,7 @@
         <v>180</v>
       </c>
       <c r="F27" s="26"/>
-      <c r="G27" s="65" t="s">
+      <c r="G27" s="40" t="s">
         <v>147</v>
       </c>
       <c r="H27" s="11">
@@ -3140,13 +3212,15 @@
       <c r="S27" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T27" s="61" t="s">
+      <c r="T27" s="38" t="s">
         <v>248</v>
       </c>
       <c r="U27" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V27" s="16"/>
+      <c r="V27" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="W27" s="16"/>
       <c r="X27" s="16"/>
     </row>
@@ -3165,7 +3239,7 @@
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="26"/>
-      <c r="G28" s="65" t="s">
+      <c r="G28" s="40" t="s">
         <v>148</v>
       </c>
       <c r="H28" s="27">
@@ -3202,13 +3276,15 @@
       <c r="S28" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T28" s="61" t="s">
+      <c r="T28" s="38" t="s">
         <v>250</v>
       </c>
       <c r="U28" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V28" s="16"/>
+      <c r="V28" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="W28" s="16"/>
       <c r="X28" s="16"/>
     </row>
@@ -3229,7 +3305,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="26"/>
-      <c r="G29" s="65" t="s">
+      <c r="G29" s="40" t="s">
         <v>10</v>
       </c>
       <c r="H29" s="11">
@@ -3256,9 +3332,8 @@
       <c r="Q29" s="24"/>
       <c r="R29" s="23"/>
       <c r="S29" s="24"/>
-      <c r="T29" s="61"/>
+      <c r="T29" s="38"/>
       <c r="U29" s="24"/>
-      <c r="V29" s="16"/>
       <c r="W29" s="16"/>
       <c r="X29" s="16"/>
     </row>
@@ -3279,7 +3354,7 @@
         <v>149</v>
       </c>
       <c r="F30" s="26"/>
-      <c r="G30" s="65" t="s">
+      <c r="G30" s="40" t="s">
         <v>149</v>
       </c>
       <c r="H30" s="27">
@@ -3316,13 +3391,15 @@
       <c r="S30" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T30" s="61" t="s">
+      <c r="T30" s="38" t="s">
         <v>249</v>
       </c>
       <c r="U30" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V30" s="16"/>
+      <c r="V30" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="W30" s="16"/>
       <c r="X30" s="16"/>
     </row>
@@ -3341,7 +3418,7 @@
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="26"/>
-      <c r="G31" s="65"/>
+      <c r="G31" s="40"/>
       <c r="H31" s="11">
         <v>29</v>
       </c>
@@ -3370,11 +3447,14 @@
       <c r="S31" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="T31" s="61" t="s">
+      <c r="T31" s="38" t="s">
         <v>251</v>
       </c>
       <c r="U31" s="24" t="s">
         <v>221</v>
+      </c>
+      <c r="V31" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="W31" s="16"/>
       <c r="X31" s="16"/>
@@ -3386,7 +3466,7 @@
       <c r="D32" s="30"/>
       <c r="E32" s="25"/>
       <c r="F32" s="26"/>
-      <c r="G32" s="65"/>
+      <c r="G32" s="40"/>
       <c r="H32" s="26"/>
       <c r="I32" s="4"/>
       <c r="J32" s="29"/>
@@ -3411,7 +3491,7 @@
       <c r="D33" s="30"/>
       <c r="E33" s="25"/>
       <c r="F33" s="26"/>
-      <c r="G33" s="66"/>
+      <c r="G33" s="41"/>
       <c r="H33" s="26"/>
       <c r="I33" s="4"/>
       <c r="J33" s="29"/>
@@ -3436,7 +3516,7 @@
       <c r="D34" s="30"/>
       <c r="E34" s="25"/>
       <c r="F34" s="26"/>
-      <c r="G34" s="66"/>
+      <c r="G34" s="41"/>
       <c r="H34" s="26"/>
       <c r="I34" s="4"/>
       <c r="J34" s="36"/>
@@ -3461,7 +3541,7 @@
       <c r="D35" s="30"/>
       <c r="E35" s="25"/>
       <c r="F35" s="26"/>
-      <c r="G35" s="66"/>
+      <c r="G35" s="41"/>
       <c r="H35" s="26"/>
       <c r="I35" s="4"/>
       <c r="J35" s="36"/>
@@ -3486,7 +3566,7 @@
       <c r="D36" s="30"/>
       <c r="E36" s="25"/>
       <c r="F36" s="26"/>
-      <c r="G36" s="66"/>
+      <c r="G36" s="41"/>
       <c r="H36" s="26"/>
       <c r="I36" s="4"/>
       <c r="J36" s="36"/>
@@ -3511,7 +3591,7 @@
       <c r="D37" s="30"/>
       <c r="E37" s="25"/>
       <c r="F37" s="26"/>
-      <c r="G37" s="66"/>
+      <c r="G37" s="41"/>
       <c r="H37" s="26"/>
       <c r="I37" s="4"/>
       <c r="J37" s="36"/>
@@ -3536,7 +3616,7 @@
       <c r="D38" s="30"/>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
-      <c r="G38" s="66"/>
+      <c r="G38" s="41"/>
       <c r="H38" s="26"/>
       <c r="I38" s="4"/>
       <c r="J38" s="36"/>
@@ -3561,7 +3641,7 @@
       <c r="D39" s="30"/>
       <c r="E39" s="25"/>
       <c r="F39" s="26"/>
-      <c r="G39" s="66"/>
+      <c r="G39" s="41"/>
       <c r="H39" s="26"/>
       <c r="I39" s="4"/>
       <c r="J39" s="36"/>
@@ -3586,7 +3666,7 @@
       <c r="D40" s="30"/>
       <c r="E40" s="25"/>
       <c r="F40" s="26"/>
-      <c r="G40" s="66"/>
+      <c r="G40" s="41"/>
       <c r="H40" s="26"/>
       <c r="I40" s="4"/>
       <c r="J40" s="36"/>
@@ -3611,7 +3691,7 @@
       <c r="D41" s="30"/>
       <c r="E41" s="25"/>
       <c r="F41" s="26"/>
-      <c r="G41" s="66"/>
+      <c r="G41" s="41"/>
       <c r="H41" s="26"/>
       <c r="I41" s="4"/>
       <c r="J41" s="36"/>
@@ -3636,7 +3716,7 @@
       <c r="D42" s="30"/>
       <c r="E42" s="25"/>
       <c r="F42" s="26"/>
-      <c r="G42" s="66"/>
+      <c r="G42" s="41"/>
       <c r="H42" s="26"/>
       <c r="I42" s="4"/>
       <c r="J42" s="36"/>
@@ -3661,7 +3741,7 @@
       <c r="D43" s="30"/>
       <c r="E43" s="25"/>
       <c r="F43" s="26"/>
-      <c r="G43" s="66"/>
+      <c r="G43" s="41"/>
       <c r="H43" s="26"/>
       <c r="I43" s="4"/>
       <c r="J43" s="36"/>
@@ -3686,7 +3766,7 @@
       <c r="D44" s="30"/>
       <c r="E44" s="25"/>
       <c r="F44" s="26"/>
-      <c r="G44" s="66"/>
+      <c r="G44" s="41"/>
       <c r="H44" s="26"/>
       <c r="I44" s="4"/>
       <c r="J44" s="36"/>
@@ -3711,7 +3791,7 @@
       <c r="D45" s="30"/>
       <c r="E45" s="25"/>
       <c r="F45" s="26"/>
-      <c r="G45" s="66"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="26"/>
       <c r="I45" s="4"/>
       <c r="J45" s="36"/>
@@ -3736,7 +3816,7 @@
       <c r="D46" s="30"/>
       <c r="E46" s="25"/>
       <c r="F46" s="26"/>
-      <c r="G46" s="66"/>
+      <c r="G46" s="41"/>
       <c r="H46" s="26"/>
       <c r="I46" s="4"/>
       <c r="J46" s="36"/>
@@ -3761,7 +3841,7 @@
       <c r="D47" s="30"/>
       <c r="E47" s="25"/>
       <c r="F47" s="26"/>
-      <c r="G47" s="66"/>
+      <c r="G47" s="41"/>
       <c r="H47" s="26"/>
       <c r="I47" s="4"/>
       <c r="J47" s="36"/>
@@ -3786,7 +3866,7 @@
       <c r="D48" s="30"/>
       <c r="E48" s="25"/>
       <c r="F48" s="26"/>
-      <c r="G48" s="66"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="26"/>
       <c r="I48" s="4"/>
       <c r="J48" s="36"/>
@@ -3811,7 +3891,7 @@
       <c r="D49" s="30"/>
       <c r="E49" s="25"/>
       <c r="F49" s="26"/>
-      <c r="G49" s="66"/>
+      <c r="G49" s="41"/>
       <c r="H49" s="26"/>
       <c r="I49" s="4"/>
       <c r="J49" s="36"/>
@@ -3836,7 +3916,7 @@
       <c r="D50" s="30"/>
       <c r="E50" s="25"/>
       <c r="F50" s="26"/>
-      <c r="G50" s="66"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="26"/>
       <c r="I50" s="4"/>
       <c r="J50" s="36"/>
@@ -3861,7 +3941,7 @@
       <c r="D51" s="30"/>
       <c r="E51" s="25"/>
       <c r="F51" s="26"/>
-      <c r="G51" s="66"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="26"/>
       <c r="I51" s="4"/>
       <c r="J51" s="36"/>
@@ -3886,7 +3966,7 @@
       <c r="D52" s="30"/>
       <c r="E52" s="25"/>
       <c r="F52" s="26"/>
-      <c r="G52" s="66"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="26"/>
       <c r="I52" s="4"/>
       <c r="J52" s="36"/>
@@ -3911,7 +3991,7 @@
       <c r="D53" s="30"/>
       <c r="E53" s="25"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="66"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="26"/>
       <c r="I53" s="4"/>
       <c r="J53" s="36"/>
@@ -3936,7 +4016,7 @@
       <c r="D54" s="30"/>
       <c r="E54" s="25"/>
       <c r="F54" s="26"/>
-      <c r="G54" s="66"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="26"/>
       <c r="I54" s="4"/>
       <c r="J54" s="36"/>
@@ -3961,7 +4041,7 @@
       <c r="D55" s="30"/>
       <c r="E55" s="25"/>
       <c r="F55" s="26"/>
-      <c r="G55" s="66"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="26"/>
       <c r="I55" s="4"/>
       <c r="J55" s="36"/>
@@ -3986,7 +4066,7 @@
       <c r="D56" s="30"/>
       <c r="E56" s="25"/>
       <c r="F56" s="26"/>
-      <c r="G56" s="66"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="26"/>
       <c r="I56" s="4"/>
       <c r="J56" s="36"/>
@@ -4011,7 +4091,7 @@
       <c r="D57" s="30"/>
       <c r="E57" s="25"/>
       <c r="F57" s="26"/>
-      <c r="G57" s="66"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="26"/>
       <c r="I57" s="4"/>
       <c r="J57" s="36"/>
@@ -4034,7 +4114,7 @@
       <c r="D58" s="30"/>
       <c r="E58" s="25"/>
       <c r="F58" s="26"/>
-      <c r="G58" s="66"/>
+      <c r="G58" s="41"/>
       <c r="H58" s="26"/>
       <c r="I58" s="4"/>
       <c r="J58" s="36"/>
@@ -4057,7 +4137,7 @@
       <c r="D59" s="30"/>
       <c r="E59" s="25"/>
       <c r="F59" s="26"/>
-      <c r="G59" s="66"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="26"/>
       <c r="I59" s="4"/>
       <c r="J59" s="36"/>
@@ -4080,7 +4160,7 @@
       <c r="D60" s="30"/>
       <c r="E60" s="25"/>
       <c r="F60" s="26"/>
-      <c r="G60" s="66"/>
+      <c r="G60" s="41"/>
       <c r="H60" s="26"/>
       <c r="I60" s="4"/>
       <c r="J60" s="36"/>
@@ -4103,7 +4183,7 @@
       <c r="D61" s="30"/>
       <c r="E61" s="25"/>
       <c r="F61" s="26"/>
-      <c r="G61" s="66"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="26"/>
       <c r="I61" s="4"/>
       <c r="J61" s="36"/>
@@ -4126,7 +4206,7 @@
       <c r="D62" s="30"/>
       <c r="E62" s="25"/>
       <c r="F62" s="26"/>
-      <c r="G62" s="66"/>
+      <c r="G62" s="41"/>
       <c r="H62" s="26"/>
       <c r="I62" s="4"/>
       <c r="J62" s="36"/>
@@ -4149,7 +4229,7 @@
       <c r="D63" s="30"/>
       <c r="E63" s="25"/>
       <c r="F63" s="26"/>
-      <c r="G63" s="66"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="26"/>
       <c r="I63" s="4"/>
       <c r="J63" s="36"/>
@@ -4172,7 +4252,7 @@
       <c r="D64" s="30"/>
       <c r="E64" s="25"/>
       <c r="F64" s="26"/>
-      <c r="G64" s="66"/>
+      <c r="G64" s="41"/>
       <c r="H64" s="26"/>
       <c r="I64" s="4"/>
       <c r="J64" s="36"/>
@@ -4195,7 +4275,7 @@
       <c r="D65" s="30"/>
       <c r="E65" s="25"/>
       <c r="F65" s="26"/>
-      <c r="G65" s="66"/>
+      <c r="G65" s="41"/>
       <c r="H65" s="26"/>
       <c r="I65" s="4"/>
       <c r="J65" s="36"/>
@@ -4218,7 +4298,7 @@
       <c r="D66" s="30"/>
       <c r="E66" s="25"/>
       <c r="F66" s="26"/>
-      <c r="G66" s="66"/>
+      <c r="G66" s="41"/>
       <c r="H66" s="26"/>
       <c r="I66" s="4"/>
       <c r="J66" s="36"/>
@@ -4241,7 +4321,7 @@
       <c r="D67" s="30"/>
       <c r="E67" s="25"/>
       <c r="F67" s="26"/>
-      <c r="G67" s="66"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="26"/>
       <c r="I67" s="4"/>
       <c r="J67" s="36"/>
@@ -4264,7 +4344,7 @@
       <c r="D68" s="30"/>
       <c r="E68" s="25"/>
       <c r="F68" s="26"/>
-      <c r="G68" s="66"/>
+      <c r="G68" s="41"/>
       <c r="H68" s="26"/>
       <c r="I68" s="4"/>
       <c r="J68" s="36"/>
@@ -4287,7 +4367,7 @@
       <c r="D69" s="30"/>
       <c r="E69" s="25"/>
       <c r="F69" s="26"/>
-      <c r="G69" s="66"/>
+      <c r="G69" s="41"/>
       <c r="H69" s="26"/>
       <c r="I69" s="4"/>
       <c r="J69" s="36"/>
@@ -4666,12 +4746,6 @@
     <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4686,11 +4760,14 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V30">
-      <formula1>$C$39:$D$39</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:X56">
       <formula1>$A$79:$A$168</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Actualizacion para segunda publicación
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion05/ESCALETA_MA_09_05_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion05/ESCALETA_MA_09_05_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS PLANETA. FERNANDA\ESCALETAS\ESCALETA_MA_09_05_CO\ESCALETA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CristhianAndres\Documents\Github\Matematicas\fuentes\contenidos\grado09\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$31</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -722,9 +722,6 @@
     <t>Las funciones lineal y afín</t>
   </si>
   <si>
-    <t>Reconoce rectas paralelas y perpendiculares</t>
-  </si>
-  <si>
     <t>Resuelve situaciones aplicando el concepto de función</t>
   </si>
   <si>
@@ -804,6 +801,9 @@
   </si>
   <si>
     <t>Actividad para identificar la pendiente de una recta a partir de la ecuación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reconoce algebraicamente las relaciones entre rectas </t>
   </si>
 </sst>
 </file>
@@ -1505,9 +1505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,7 +1715,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>20</v>
@@ -1770,7 +1770,7 @@
       <c r="E5" s="25"/>
       <c r="F5" s="26"/>
       <c r="G5" s="40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H5" s="11">
         <v>3</v>
@@ -2084,7 +2084,7 @@
       <c r="E10" s="25"/>
       <c r="F10" s="26"/>
       <c r="G10" s="40" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="H10" s="11">
         <v>8</v>
@@ -2148,7 +2148,7 @@
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
       <c r="G11" s="40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H11" s="11">
         <v>9</v>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H12" s="11">
         <v>10</v>
@@ -2223,7 +2223,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>19</v>
@@ -2276,7 +2276,7 @@
       <c r="E13" s="25"/>
       <c r="F13" s="26"/>
       <c r="G13" s="40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H13" s="11">
         <v>11</v>
@@ -2285,7 +2285,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>20</v>
@@ -2413,7 +2413,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>20</v>
@@ -2477,7 +2477,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>20</v>
@@ -2532,7 +2532,7 @@
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
       <c r="G17" s="40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H17" s="11">
         <v>15</v>
@@ -2541,7 +2541,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>20</v>
@@ -2596,7 +2596,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
       <c r="G18" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H18" s="11">
         <v>16</v>
@@ -2660,7 +2660,7 @@
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
       <c r="G19" s="40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H19" s="11">
         <v>17</v>
@@ -2724,7 +2724,7 @@
       <c r="E20" s="25"/>
       <c r="F20" s="26"/>
       <c r="G20" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H20" s="11">
         <v>18</v>
@@ -2733,7 +2733,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>20</v>
@@ -2788,7 +2788,7 @@
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
       <c r="G21" s="40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H21" s="11">
         <v>19</v>
@@ -2797,7 +2797,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>20</v>
@@ -2863,7 +2863,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>20</v>
@@ -2918,7 +2918,7 @@
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
       <c r="G23" s="40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H23" s="11">
         <v>21</v>
@@ -2927,7 +2927,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>20</v>
@@ -2991,7 +2991,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>20</v>
@@ -3110,7 +3110,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
       <c r="G26" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H26" s="11">
         <v>24</v>
@@ -3119,7 +3119,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>20</v>
@@ -3176,7 +3176,7 @@
       </c>
       <c r="F27" s="26"/>
       <c r="G27" s="40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H27" s="11">
         <v>25</v>
@@ -3185,7 +3185,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>20</v>
@@ -3240,7 +3240,7 @@
       <c r="E28" s="25"/>
       <c r="F28" s="26"/>
       <c r="G28" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -3249,7 +3249,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K28" s="6" t="s">
         <v>20</v>

</xml_diff>